<commit_message>
Filtered terr herb and marine mammals
</commit_message>
<xml_diff>
--- a/resultFile_1.xlsx
+++ b/resultFile_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,26 +479,31 @@
           <t>δ18O carb</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>δ18O phos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sea otter</t>
+          <t>aurochs</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hb 19</t>
+          <t>Hb 47</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>terrestrial, aquatic</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -507,37 +512,40 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>-19.17</v>
+        <v>-20.51</v>
       </c>
       <c r="G2" t="n">
-        <v>11.21</v>
+        <v>10.48</v>
       </c>
       <c r="H2" t="n">
-        <v>-14.81</v>
+        <v>-10.94</v>
       </c>
       <c r="I2" t="n">
-        <v>-9.460000000000001</v>
+        <v>-7.6</v>
+      </c>
+      <c r="J2" t="n">
+        <v>17.25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sea otter</t>
+          <t>aurochs</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Hb 20</t>
+          <t>Hb 48</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>terrestrial, aquatic</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -546,76 +554,82 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>-19.88</v>
+        <v>-21.82</v>
       </c>
       <c r="G3" t="n">
-        <v>13.81</v>
+        <v>4.03</v>
       </c>
       <c r="H3" t="n">
-        <v>-16.27</v>
+        <v>-12.16</v>
       </c>
       <c r="I3" t="n">
-        <v>-9.91</v>
+        <v>-8.949999999999999</v>
+      </c>
+      <c r="J3" t="n">
+        <v>17.78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sea otter</t>
+          <t>fallow deer</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>32 FO1Hepi</t>
+          <t>S 6</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>terrestrial, aquatic</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Haithabu</t>
+          <t>Schleswig</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>-14.15</v>
+        <v>-22.82</v>
       </c>
       <c r="G4" t="n">
-        <v>13.14</v>
+        <v>9.43</v>
       </c>
       <c r="H4" t="n">
-        <v>-6.75</v>
+        <v>-11.52</v>
       </c>
       <c r="I4" t="n">
-        <v>-6.99</v>
+        <v>-9.359999999999999</v>
+      </c>
+      <c r="J4" t="n">
+        <v>17.28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sea otter</t>
+          <t>squirrel</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>33 FO2H</t>
+          <t>Hb 7</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>terrestrial, aquatic</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,76 +638,82 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>-20.63</v>
+        <v>-21.27</v>
       </c>
       <c r="G5" t="n">
-        <v>13.54</v>
+        <v>2.91</v>
       </c>
       <c r="H5" t="n">
-        <v>-15.43</v>
+        <v>-14.64</v>
       </c>
       <c r="I5" t="n">
-        <v>-7.96</v>
+        <v>-8.029999999999999</v>
+      </c>
+      <c r="J5" t="n">
+        <v>16.54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>moose</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>S 17</t>
+          <t>Hb 46</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Schleswig</t>
+          <t>Haithabu</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>-14.51</v>
+        <v>-21.5</v>
       </c>
       <c r="G6" t="n">
-        <v>12.93</v>
+        <v>4.86</v>
       </c>
       <c r="H6" t="n">
-        <v>-9.76</v>
+        <v>-11.36</v>
       </c>
       <c r="I6" t="n">
-        <v>-8.859999999999999</v>
+        <v>-7.01</v>
+      </c>
+      <c r="J6" t="n">
+        <v>17.64</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>20 KR1Ph</t>
+          <t>Hb 1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -702,37 +722,40 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>-15.09</v>
+        <v>-22.54</v>
       </c>
       <c r="G7" t="n">
-        <v>15.06</v>
+        <v>6.17</v>
       </c>
       <c r="H7" t="n">
-        <v>-11.57</v>
+        <v>-12.45</v>
       </c>
       <c r="I7" t="n">
-        <v>-7.8</v>
+        <v>-8.85</v>
+      </c>
+      <c r="J7" t="n">
+        <v>15.84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21 KR2T</t>
+          <t>Hb 2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -741,37 +764,40 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>-16.24</v>
+        <v>-21.2</v>
       </c>
       <c r="G8" t="n">
-        <v>12.8</v>
+        <v>3.8</v>
       </c>
       <c r="H8" t="n">
-        <v>-11.98</v>
+        <v>-10.8</v>
       </c>
       <c r="I8" t="n">
-        <v>-7.97</v>
+        <v>-8.220000000000001</v>
+      </c>
+      <c r="J8" t="n">
+        <v>17.04</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>22 KR3S</t>
+          <t>Hb 3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -780,37 +806,40 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>-16.31</v>
+        <v>-21.67</v>
       </c>
       <c r="G9" t="n">
-        <v>13.06</v>
+        <v>4.54</v>
       </c>
       <c r="H9" t="n">
-        <v>-9.949999999999999</v>
+        <v>-9.76</v>
       </c>
       <c r="I9" t="n">
-        <v>-7.67</v>
+        <v>-6.85</v>
+      </c>
+      <c r="J9" t="n">
+        <v>17.26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23 KR4V</t>
+          <t>Hb 5</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -819,76 +848,82 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>-16.22</v>
+        <v>-22.15</v>
       </c>
       <c r="G10" t="n">
-        <v>12.88</v>
+        <v>4.02</v>
       </c>
       <c r="H10" t="n">
-        <v>-12.96</v>
+        <v>-15.83</v>
       </c>
       <c r="I10" t="n">
-        <v>-8.449999999999999</v>
+        <v>-8.359999999999999</v>
+      </c>
+      <c r="J10" t="n">
+        <v>16.47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>24 KR5Mt</t>
+          <t>S 24</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Haithabu</t>
+          <t>Schleswig</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>-15.06</v>
+        <v>-22.38</v>
       </c>
       <c r="G11" t="n">
-        <v>13.48</v>
+        <v>4.04</v>
       </c>
       <c r="H11" t="n">
-        <v>-9.369999999999999</v>
+        <v>-11.3</v>
       </c>
       <c r="I11" t="n">
-        <v>-8.52</v>
+        <v>-7.43</v>
+      </c>
+      <c r="J11" t="n">
+        <v>17.29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>71 KR1BuTy</t>
+          <t>S 25</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -897,37 +932,40 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>-15.61</v>
+        <v>-22.78</v>
       </c>
       <c r="G12" t="n">
-        <v>12.87</v>
+        <v>5.32</v>
       </c>
       <c r="H12" t="n">
-        <v>-9.16</v>
+        <v>-13.12</v>
       </c>
       <c r="I12" t="n">
-        <v>-11.52</v>
+        <v>-10.04</v>
+      </c>
+      <c r="J12" t="n">
+        <v>16.67</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>72 KR2Sc</t>
+          <t>S 26</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -936,37 +974,40 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>-15.41</v>
+        <v>-22.39</v>
       </c>
       <c r="G13" t="n">
-        <v>12.89</v>
+        <v>3.96</v>
       </c>
       <c r="H13" t="n">
-        <v>-12.03</v>
+        <v>-13.59</v>
       </c>
       <c r="I13" t="n">
-        <v>-10.21</v>
+        <v>-9.27</v>
+      </c>
+      <c r="J13" t="n">
+        <v>14.68</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>73 KR3Mt</t>
+          <t>S 27</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -975,37 +1016,40 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>-17.22</v>
+        <v>-22.45</v>
       </c>
       <c r="G14" t="n">
-        <v>15.33</v>
+        <v>3.89</v>
       </c>
       <c r="H14" t="n">
-        <v>-13.59</v>
+        <v>-14.84</v>
       </c>
       <c r="I14" t="n">
-        <v>-11.93</v>
+        <v>-7.82</v>
+      </c>
+      <c r="J14" t="n">
+        <v>15.63</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>European hare</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>74 KR4Fi</t>
+          <t>S 28</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1014,32 +1058,35 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>-15.37</v>
+        <v>-23.4</v>
       </c>
       <c r="G15" t="n">
-        <v>12.42</v>
+        <v>4.35</v>
       </c>
       <c r="H15" t="n">
-        <v>-11.6</v>
+        <v>-15.14</v>
       </c>
       <c r="I15" t="n">
-        <v>-9.93</v>
+        <v>-6.27</v>
+      </c>
+      <c r="J15" t="n">
+        <v>17.03</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>grey seal</t>
+          <t>sea otter</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>75 KR5Mt</t>
+          <t>Hb 19</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>brackish, marine</t>
+          <t>terrestrial, aquatic</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1049,41 +1096,44 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Schleswig</t>
+          <t>Haithabu</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>-14.61</v>
+        <v>-19.17</v>
       </c>
       <c r="G16" t="n">
-        <v>13.45</v>
+        <v>11.21</v>
       </c>
       <c r="H16" t="n">
-        <v>-10.61</v>
+        <v>-14.81</v>
       </c>
       <c r="I16" t="n">
-        <v>-8.15</v>
+        <v>-9.460000000000001</v>
+      </c>
+      <c r="J16" t="n">
+        <v>15.6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>sperm whale</t>
+          <t>sea otter</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Hb 50</t>
+          <t>Hb 20</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Salzwasser</t>
+          <t>terrestrial, aquatic</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>molluscivorous</t>
+          <t>piscivorous</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1092,110 +1142,119 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>-19.34</v>
+        <v>-19.88</v>
       </c>
       <c r="G17" t="n">
-        <v>8.33</v>
+        <v>13.81</v>
       </c>
       <c r="H17" t="n">
-        <v>-14.48</v>
+        <v>-16.27</v>
       </c>
       <c r="I17" t="n">
-        <v>-5.75</v>
+        <v>-9.91</v>
+      </c>
+      <c r="J17" t="n">
+        <v>14.92</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ringed seal</t>
+          <t>European rabbit</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hb 28</t>
+          <t>S 29</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Salzwasser</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Haithabu</t>
+          <t>Schleswig</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>-12.54</v>
+        <v>-22.33</v>
       </c>
       <c r="G18" t="n">
-        <v>15.24</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="H18" t="n">
-        <v>-8.130000000000001</v>
+        <v>-11.77</v>
       </c>
       <c r="I18" t="n">
-        <v>-8.880000000000001</v>
+        <v>-6.95</v>
+      </c>
+      <c r="J18" t="n">
+        <v>16.64</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>saddleback seal</t>
+          <t>European rabbit</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hb 30</t>
+          <t>S 30</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Haithabu</t>
+          <t>Schleswig</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>-15.98</v>
+        <v>-21.91</v>
       </c>
       <c r="G19" t="n">
-        <v>11.21</v>
+        <v>10.98</v>
       </c>
       <c r="H19" t="n">
-        <v>-9.35</v>
+        <v>-10.47</v>
       </c>
       <c r="I19" t="n">
-        <v>-7.54</v>
+        <v>-8.220000000000001</v>
+      </c>
+      <c r="J19" t="n">
+        <v>16.52</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>saddleback seal</t>
+          <t>grey seal</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>KHb 25</t>
+          <t>S 17</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>marine</t>
+          <t>brackish, marine</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1205,41 +1264,44 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Haithabu</t>
+          <t>Schleswig</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>-16.67</v>
+        <v>-14.51</v>
       </c>
       <c r="G20" t="n">
-        <v>12.46</v>
+        <v>12.93</v>
       </c>
       <c r="H20" t="n">
-        <v>-11.13</v>
+        <v>-9.76</v>
       </c>
       <c r="I20" t="n">
-        <v>-7.99</v>
+        <v>-8.859999999999999</v>
+      </c>
+      <c r="J20" t="n">
+        <v>16.87</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>saddleback seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>26 SR2Fi</t>
+          <t>Hb 83</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1248,37 +1310,40 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>-16.65</v>
+        <v>-22.15</v>
       </c>
       <c r="G21" t="n">
-        <v>12.23</v>
+        <v>5.73</v>
       </c>
       <c r="H21" t="n">
-        <v>-8.4</v>
+        <v>-11</v>
       </c>
       <c r="I21" t="n">
-        <v>-12.81</v>
+        <v>-7.87</v>
+      </c>
+      <c r="J21" t="n">
+        <v>16.85</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Hb 23</t>
+          <t>Hb 84</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1287,37 +1352,40 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>-20.7</v>
+        <v>-22.54</v>
       </c>
       <c r="G22" t="n">
-        <v>8.630000000000001</v>
+        <v>4.17</v>
       </c>
       <c r="H22" t="n">
-        <v>-11.22</v>
+        <v>-11.47</v>
       </c>
       <c r="I22" t="n">
-        <v>-8.73</v>
+        <v>-8.09</v>
+      </c>
+      <c r="J22" t="n">
+        <v>16.03</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Hb 24</t>
+          <t>Hb 85</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1326,37 +1394,40 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>-13.71</v>
+        <v>-21.83</v>
       </c>
       <c r="G23" t="n">
-        <v>13.08</v>
+        <v>6.74</v>
       </c>
       <c r="H23" t="n">
-        <v>-7.67</v>
+        <v>-11.84</v>
       </c>
       <c r="I23" t="n">
-        <v>-8.91</v>
+        <v>-8.5</v>
+      </c>
+      <c r="J23" t="n">
+        <v>17.05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Hb 25</t>
+          <t>Hb 86</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1365,37 +1436,40 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>-16.96</v>
+        <v>-21.86</v>
       </c>
       <c r="G24" t="n">
-        <v>12</v>
+        <v>5.63</v>
       </c>
       <c r="H24" t="n">
-        <v>-10.8</v>
+        <v>-10.86</v>
       </c>
       <c r="I24" t="n">
-        <v>-9.119999999999999</v>
+        <v>-6.88</v>
+      </c>
+      <c r="J24" t="n">
+        <v>17.41</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Hb 26</t>
+          <t>Hb 87</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1404,37 +1478,40 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>-15.98</v>
+        <v>-22.14</v>
       </c>
       <c r="G25" t="n">
-        <v>13.18</v>
+        <v>4.95</v>
       </c>
       <c r="H25" t="n">
-        <v>-6.23</v>
+        <v>-12.11</v>
       </c>
       <c r="I25" t="n">
-        <v>-10.18</v>
+        <v>-9.210000000000001</v>
+      </c>
+      <c r="J25" t="n">
+        <v>16.49</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Hb 27</t>
+          <t>Hb 88</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1443,37 +1520,40 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>-13.41</v>
+        <v>-22.25</v>
       </c>
       <c r="G26" t="n">
-        <v>16.96</v>
+        <v>4.91</v>
       </c>
       <c r="H26" t="n">
-        <v>-9.710000000000001</v>
+        <v>-14.51</v>
       </c>
       <c r="I26" t="n">
-        <v>-8.970000000000001</v>
+        <v>-8.029999999999999</v>
+      </c>
+      <c r="J26" t="n">
+        <v>16.71</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>KHb 30</t>
+          <t>Hb 89</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1482,37 +1562,40 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>-17.01</v>
+        <v>-22</v>
       </c>
       <c r="G27" t="n">
-        <v>11.99</v>
+        <v>4.98</v>
       </c>
       <c r="H27" t="n">
-        <v>-9.49</v>
+        <v>-13.17</v>
       </c>
       <c r="I27" t="n">
-        <v>-9.619999999999999</v>
+        <v>-7.18</v>
+      </c>
+      <c r="J27" t="n">
+        <v>17.2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KHb 31</t>
+          <t>Hb 90</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1521,37 +1604,40 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>-13.5</v>
+        <v>-21.69</v>
       </c>
       <c r="G28" t="n">
-        <v>14.52</v>
+        <v>6.39</v>
       </c>
       <c r="H28" t="n">
-        <v>-9.57</v>
+        <v>-14.35</v>
       </c>
       <c r="I28" t="n">
-        <v>-13.51</v>
+        <v>-6.93</v>
+      </c>
+      <c r="J28" t="n">
+        <v>17.44</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>27 SH1Ph</t>
+          <t>Hb 91</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1560,37 +1646,40 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>-14.78</v>
+        <v>-21.36</v>
       </c>
       <c r="G29" t="n">
-        <v>14.2</v>
+        <v>5.82</v>
       </c>
       <c r="H29" t="n">
-        <v>-10.4</v>
+        <v>-12.98</v>
       </c>
       <c r="I29" t="n">
-        <v>-6.63</v>
+        <v>-7.23</v>
+      </c>
+      <c r="J29" t="n">
+        <v>18.53</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>28 SH2R</t>
+          <t>Hb 92</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>terrestrial</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>herbivorous</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1599,37 +1688,40 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>-14.94</v>
+        <v>-22.23</v>
       </c>
       <c r="G30" t="n">
-        <v>15.29</v>
+        <v>6.01</v>
       </c>
       <c r="H30" t="n">
-        <v>-6.77</v>
+        <v>-13.87</v>
       </c>
       <c r="I30" t="n">
-        <v>-6.5</v>
+        <v>-8.01</v>
+      </c>
+      <c r="J30" t="n">
+        <v>15.77</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>common seal</t>
+          <t>sperm whale</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>29 SH3V</t>
+          <t>Hb 50</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>freshwater, brackish, marine</t>
+          <t>Salzwasser</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>piscivorous</t>
+          <t>molluscivorous</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1638,55 +1730,1573 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>-15</v>
+        <v>-19.34</v>
       </c>
       <c r="G31" t="n">
-        <v>11.96</v>
+        <v>8.33</v>
       </c>
       <c r="H31" t="n">
-        <v>-7.98</v>
+        <v>-14.48</v>
       </c>
       <c r="I31" t="n">
-        <v>-5.74</v>
+        <v>-5.75</v>
+      </c>
+      <c r="J31" t="n">
+        <v>19.59</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>walrus</t>
+          <t>roe deer</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>KS 76</t>
+          <t>Hb 40</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>-24</v>
+      </c>
+      <c r="G32" t="n">
+        <v>5.38</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-15.79</v>
+      </c>
+      <c r="I32" t="n">
+        <v>-10.06</v>
+      </c>
+      <c r="J32" t="n">
+        <v>16.57</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>roe deer</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Hb 41</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>-21.95</v>
+      </c>
+      <c r="G33" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="H33" t="n">
+        <v>-13.63</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-8.92</v>
+      </c>
+      <c r="J33" t="n">
+        <v>16.79</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>roe deer</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Hb 42</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>-22.67</v>
+      </c>
+      <c r="G34" t="n">
+        <v>4.82</v>
+      </c>
+      <c r="H34" t="n">
+        <v>-15.01</v>
+      </c>
+      <c r="I34" t="n">
+        <v>-8.31</v>
+      </c>
+      <c r="J34" t="n">
+        <v>16.41</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>roe deer</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Hb 43</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>-22.41</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H35" t="n">
+        <v>-15.6</v>
+      </c>
+      <c r="I35" t="n">
+        <v>-7.51</v>
+      </c>
+      <c r="J35" t="n">
+        <v>16.91</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>roe deer</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>S 8</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Schleswig</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>-21.94</v>
+      </c>
+      <c r="G36" t="n">
+        <v>4.58</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-14.55</v>
+      </c>
+      <c r="I36" t="n">
+        <v>-9.48</v>
+      </c>
+      <c r="J36" t="n">
+        <v>16.47</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>roe deer</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>S 9</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Schleswig</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>-21.73</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="H37" t="n">
+        <v>-13.33</v>
+      </c>
+      <c r="I37" t="n">
+        <v>-9.630000000000001</v>
+      </c>
+      <c r="J37" t="n">
+        <v>16.4</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>roe deer</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>S 11</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Schleswig</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>-20.07</v>
+      </c>
+      <c r="G38" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-11.89</v>
+      </c>
+      <c r="I38" t="n">
+        <v>-7.97</v>
+      </c>
+      <c r="J38" t="n">
+        <v>16.69</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>roe deer</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>S 12</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Schleswig</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>-22.78</v>
+      </c>
+      <c r="G39" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="H39" t="n">
+        <v>-14.53</v>
+      </c>
+      <c r="I39" t="n">
+        <v>-8.5</v>
+      </c>
+      <c r="J39" t="n">
+        <v>16.65</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Hb 53</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>-21.46</v>
+      </c>
+      <c r="G40" t="n">
+        <v>4.39</v>
+      </c>
+      <c r="H40" t="n">
+        <v>-9.970000000000001</v>
+      </c>
+      <c r="I40" t="n">
+        <v>-7.14</v>
+      </c>
+      <c r="J40" t="n">
+        <v>16.71</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Hb 54</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>-21.62</v>
+      </c>
+      <c r="G41" t="n">
+        <v>4.89</v>
+      </c>
+      <c r="H41" t="n">
+        <v>-10.62</v>
+      </c>
+      <c r="I41" t="n">
+        <v>-6.84</v>
+      </c>
+      <c r="J41" t="n">
+        <v>16.88</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Hb 55</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>-22.48</v>
+      </c>
+      <c r="G42" t="n">
+        <v>6.69</v>
+      </c>
+      <c r="H42" t="n">
+        <v>-11.86</v>
+      </c>
+      <c r="I42" t="n">
+        <v>-7.07</v>
+      </c>
+      <c r="J42" t="n">
+        <v>17.18</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Hb 56</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>-21.61</v>
+      </c>
+      <c r="G43" t="n">
+        <v>5.18</v>
+      </c>
+      <c r="H43" t="n">
+        <v>-10.51</v>
+      </c>
+      <c r="I43" t="n">
+        <v>-7.15</v>
+      </c>
+      <c r="J43" t="n">
+        <v>17.07</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Hb 57</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>-21.67</v>
+      </c>
+      <c r="G44" t="n">
+        <v>5.53</v>
+      </c>
+      <c r="H44" t="n">
+        <v>-10.67</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-6.43</v>
+      </c>
+      <c r="J44" t="n">
+        <v>18.14</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Hb 58</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>-21.44</v>
+      </c>
+      <c r="G45" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="H45" t="n">
+        <v>-9.98</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-7.27</v>
+      </c>
+      <c r="J45" t="n">
+        <v>17.66</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Hb 59</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>-21.67</v>
+      </c>
+      <c r="G46" t="n">
+        <v>4.98</v>
+      </c>
+      <c r="H46" t="n">
+        <v>-10.8</v>
+      </c>
+      <c r="I46" t="n">
+        <v>-6.88</v>
+      </c>
+      <c r="J46" t="n">
+        <v>17.51</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Hb 60</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>-21.91</v>
+      </c>
+      <c r="G47" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="H47" t="n">
+        <v>-9.9</v>
+      </c>
+      <c r="I47" t="n">
+        <v>-7.03</v>
+      </c>
+      <c r="J47" t="n">
+        <v>17.62</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Hb 61</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>-21.28</v>
+      </c>
+      <c r="G48" t="n">
+        <v>4.58</v>
+      </c>
+      <c r="H48" t="n">
+        <v>-9.93</v>
+      </c>
+      <c r="I48" t="n">
+        <v>-7.44</v>
+      </c>
+      <c r="J48" t="n">
+        <v>17.13</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>cattle</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Hb 62</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>-21.62</v>
+      </c>
+      <c r="G49" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="H49" t="n">
+        <v>-11.2</v>
+      </c>
+      <c r="I49" t="n">
+        <v>-7.37</v>
+      </c>
+      <c r="J49" t="n">
+        <v>17.18</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ringed seal</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Hb 28</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Salzwasser</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>piscivorous</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>-12.54</v>
+      </c>
+      <c r="G50" t="n">
+        <v>15.24</v>
+      </c>
+      <c r="H50" t="n">
+        <v>-8.130000000000001</v>
+      </c>
+      <c r="I50" t="n">
+        <v>-8.880000000000001</v>
+      </c>
+      <c r="J50" t="n">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>red deer</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Hb 35</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>-22.03</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="H51" t="n">
+        <v>-11.36</v>
+      </c>
+      <c r="I51" t="n">
+        <v>-8.390000000000001</v>
+      </c>
+      <c r="J51" t="n">
+        <v>17.6</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>red deer</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Hb 36</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>-22.09</v>
+      </c>
+      <c r="G52" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="H52" t="n">
+        <v>-14.08</v>
+      </c>
+      <c r="I52" t="n">
+        <v>-7.37</v>
+      </c>
+      <c r="J52" t="n">
+        <v>16.71</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>red deer</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Hb 38</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>-22.74</v>
+      </c>
+      <c r="G53" t="n">
+        <v>5.84</v>
+      </c>
+      <c r="H53" t="n">
+        <v>-13.03</v>
+      </c>
+      <c r="I53" t="n">
+        <v>-7.67</v>
+      </c>
+      <c r="J53" t="n">
+        <v>16.38</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>red deer</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Hb 39</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>-22.05</v>
+      </c>
+      <c r="G54" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="H54" t="n">
+        <v>-12.28</v>
+      </c>
+      <c r="I54" t="n">
+        <v>-8.34</v>
+      </c>
+      <c r="J54" t="n">
+        <v>16.54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>red deer</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>S 1</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Schleswig</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>-21.53</v>
+      </c>
+      <c r="G55" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="H55" t="n">
+        <v>-13.1</v>
+      </c>
+      <c r="I55" t="n">
+        <v>-7.87</v>
+      </c>
+      <c r="J55" t="n">
+        <v>17.41</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>red deer</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>S 2</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Schleswig</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>-22.27</v>
+      </c>
+      <c r="G56" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="H56" t="n">
+        <v>-14.09</v>
+      </c>
+      <c r="I56" t="n">
+        <v>-8.17</v>
+      </c>
+      <c r="J56" t="n">
+        <v>17.03</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>red deer</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>S 3</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Schleswig</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>-23.05</v>
+      </c>
+      <c r="G57" t="n">
+        <v>5.81</v>
+      </c>
+      <c r="H57" t="n">
+        <v>-15.19</v>
+      </c>
+      <c r="I57" t="n">
+        <v>-8.869999999999999</v>
+      </c>
+      <c r="J57" t="n">
+        <v>16.53</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>red deer</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>S 5</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Schleswig</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>-22.69</v>
+      </c>
+      <c r="G58" t="n">
+        <v>5.51</v>
+      </c>
+      <c r="H58" t="n">
+        <v>-14.65</v>
+      </c>
+      <c r="I58" t="n">
+        <v>-8.140000000000001</v>
+      </c>
+      <c r="J58" t="n">
+        <v>17.32</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>saddleback seal</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Hb 30</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>marine</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>molluscivorous</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Schleswig</t>
-        </is>
-      </c>
-      <c r="F32" t="n">
-        <v>-14</v>
-      </c>
-      <c r="G32" t="n">
-        <v>12.32</v>
-      </c>
-      <c r="H32" t="n">
-        <v>-8.699999999999999</v>
-      </c>
-      <c r="I32" t="n">
-        <v>-6.33</v>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>piscivorous</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>-15.98</v>
+      </c>
+      <c r="G59" t="n">
+        <v>11.21</v>
+      </c>
+      <c r="H59" t="n">
+        <v>-9.35</v>
+      </c>
+      <c r="I59" t="n">
+        <v>-7.54</v>
+      </c>
+      <c r="J59" t="n">
+        <v>15.04</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>sheep</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Hb 73</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>-21.45</v>
+      </c>
+      <c r="G60" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="H60" t="n">
+        <v>-10.11</v>
+      </c>
+      <c r="I60" t="n">
+        <v>-7</v>
+      </c>
+      <c r="J60" t="n">
+        <v>19.73</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>sheep</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Hb 74</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>-21.82</v>
+      </c>
+      <c r="G61" t="n">
+        <v>7.49</v>
+      </c>
+      <c r="H61" t="n">
+        <v>-12.06</v>
+      </c>
+      <c r="I61" t="n">
+        <v>-8.890000000000001</v>
+      </c>
+      <c r="J61" t="n">
+        <v>16.68</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>sheep</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Hb 76</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>-21.49</v>
+      </c>
+      <c r="G62" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="H62" t="n">
+        <v>-10.09</v>
+      </c>
+      <c r="I62" t="n">
+        <v>-5.79</v>
+      </c>
+      <c r="J62" t="n">
+        <v>19.72</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>sheep</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Hb 77</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>-21.6</v>
+      </c>
+      <c r="G63" t="n">
+        <v>6.16</v>
+      </c>
+      <c r="H63" t="n">
+        <v>-9.49</v>
+      </c>
+      <c r="I63" t="n">
+        <v>-5.32</v>
+      </c>
+      <c r="J63" t="n">
+        <v>19.64</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>sheep</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Hb 78</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>-22.29</v>
+      </c>
+      <c r="G64" t="n">
+        <v>7.55</v>
+      </c>
+      <c r="H64" t="n">
+        <v>-11.3</v>
+      </c>
+      <c r="I64" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="J64" t="n">
+        <v>18.32</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>sheep</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Hb 79</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>terrestrial</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>herbivorous</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>-20.95</v>
+      </c>
+      <c r="G65" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="H65" t="n">
+        <v>-10.65</v>
+      </c>
+      <c r="I65" t="n">
+        <v>-5.14</v>
+      </c>
+      <c r="J65" t="n">
+        <v>17.92</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>common seal</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Hb 23</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>freshwater, brackish, marine</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>piscivorous</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>-20.7</v>
+      </c>
+      <c r="G66" t="n">
+        <v>8.630000000000001</v>
+      </c>
+      <c r="H66" t="n">
+        <v>-11.22</v>
+      </c>
+      <c r="I66" t="n">
+        <v>-8.73</v>
+      </c>
+      <c r="J66" t="n">
+        <v>17.21</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>common seal</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Hb 26</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>freshwater, brackish, marine</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>piscivorous</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>-15.98</v>
+      </c>
+      <c r="G67" t="n">
+        <v>13.18</v>
+      </c>
+      <c r="H67" t="n">
+        <v>-6.23</v>
+      </c>
+      <c r="I67" t="n">
+        <v>-10.18</v>
+      </c>
+      <c r="J67" t="n">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>common seal</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Hb 27</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>freshwater, brackish, marine</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>piscivorous</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Haithabu</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>-13.41</v>
+      </c>
+      <c r="G68" t="n">
+        <v>16.96</v>
+      </c>
+      <c r="H68" t="n">
+        <v>-9.710000000000001</v>
+      </c>
+      <c r="I68" t="n">
+        <v>-8.970000000000001</v>
+      </c>
+      <c r="J68" t="n">
+        <v>15.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>